<commit_message>
detecta quan es FULL_CHANGE i no DELETE
</commit_message>
<xml_diff>
--- a/src/excelB.xlsx
+++ b/src/excelB.xlsx
@@ -38,12 +38,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+  <fonts count="16">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -60,16 +59,135 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -77,8 +195,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -102,6 +235,57 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -109,14 +293,91 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -125,10 +386,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -153,154 +414,340 @@
       <c r="A5" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="B8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="B9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="B10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="B11" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="B12" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>9</v>
       </c>
+      <c r="B13" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="B14" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="B15" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="B16" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="B17" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>15</v>
       </c>
+      <c r="B18" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="B19" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>17</v>
       </c>
+      <c r="B20" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>118</v>
       </c>
+      <c r="B21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>19</v>
       </c>
+      <c r="B22" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="B23" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>21</v>
       </c>
+      <c r="B24" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>22</v>
       </c>
+      <c r="B25" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>23</v>
       </c>
+      <c r="B26" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="B27" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>25</v>
       </c>
+      <c r="B28" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>26</v>
       </c>
+      <c r="B29" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>27</v>
       </c>
+      <c r="B30" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>28</v>
       </c>
+      <c r="B31" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>29</v>
       </c>
+      <c r="B32" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B33" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>31</v>
       </c>
+      <c r="B34" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="C35" s="0" t="n">
         <v>32</v>
       </c>
     </row>

</xml_diff>